<commit_message>
Cambios en finalizar pedidos
</commit_message>
<xml_diff>
--- a/Tareas miscompras.xlsx
+++ b/Tareas miscompras.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aprendizaje\Cursos Actuales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\demoProyects\FrontEndMisCompras\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2F01F0-B05B-4348-B4B0-09F325FA26A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20070" windowHeight="7518"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20070" windowHeight="7515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Prioridad</t>
   </si>
@@ -91,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -479,20 +475,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="89.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -503,7 +499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -514,7 +510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -525,7 +521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -536,7 +532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -547,7 +543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -558,7 +554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -569,7 +565,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -578,42 +574,45 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Se completo proceso de pedido
</commit_message>
<xml_diff>
--- a/Tareas miscompras.xlsx
+++ b/Tareas miscompras.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\demoProyects\FrontEndMisCompras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2019\Ventas\FrontEndMisCompras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2F01F0-B05B-4348-B4B0-09F325FA26A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20070" windowHeight="7515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20070" windowHeight="7518"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Prioridad</t>
   </si>
@@ -87,7 +86,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -475,20 +474,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="89.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -499,7 +498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -510,7 +509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -521,7 +520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -532,7 +531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -543,7 +542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -554,7 +553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -565,7 +564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -574,7 +573,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
@@ -582,37 +581,43 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="3" t="s">
         <v>18</v>
       </c>

</xml_diff>